<commit_message>
Add schedule device status warning
</commit_message>
<xml_diff>
--- a/Services/Server/Server.API/wwwroot/Reports/BAOCAOTRANGTHAITHIETBI.xlsx
+++ b/Services/Server/Server.API/wwwroot/Reports/BAOCAOTRANGTHAITHIETBI.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACS Solutions\Projects\AMMS_DiemDanhHocSinh\Services\Server\Server.API\wwwroot\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9891C4-763F-4AA6-BA32-DBCD702E5564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69455AE-B9E3-44DD-88AF-540505C7E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="192" windowWidth="18000" windowHeight="12048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thiết bị Offline" sheetId="1" r:id="rId1"/>
     <sheet name="Thiết bị Online" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="datas">'Thiết bị Online'!$A$10:$I$11</definedName>
-    <definedName name="items">'Thiết bị Offline'!$A$10:$I$11</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Thiết bị Offline'!$A$1:$O$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Thiết bị Online'!$A$1:$J$21</definedName>
+    <definedName name="datas">'Thiết bị Online'!$A$10:$H$11</definedName>
+    <definedName name="items">'Thiết bị Offline'!$A$10:$H$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Thiết bị Offline'!$A$1:$N$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Thiết bị Online'!$A$1:$I$21</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>N0.</t>
   </si>
@@ -111,22 +111,10 @@
     <t>{{item.SerialNumber}}</t>
   </si>
   <si>
-    <t>{{item.LastTimeUpdateSocket}}</t>
-  </si>
-  <si>
     <t>{{item.OrganizationName}}</t>
   </si>
   <si>
-    <t>WanIpAddress</t>
-  </si>
-  <si>
-    <t>{{item.WanIpAddress}}</t>
-  </si>
-  <si>
     <t>IpAddress</t>
-  </si>
-  <si>
-    <t>{{item.IpAddress}}</t>
   </si>
   <si>
     <r>
@@ -165,6 +153,9 @@
   </si>
   <si>
     <t>{{item.DeviceModel}}</t>
+  </si>
+  <si>
+    <t>{{item.CheckConnectTime}}</t>
   </si>
 </sst>
 </file>
@@ -602,10 +593,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I65538"/>
+  <dimension ref="A2:H65538"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -616,12 +607,12 @@
     <col min="4" max="4" width="19.81640625" style="2" customWidth="1"/>
     <col min="5" max="6" width="31.1796875" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.1796875" style="10" customWidth="1"/>
-    <col min="8" max="9" width="23.90625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="2.1796875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="3"/>
+    <col min="8" max="8" width="23.90625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.1796875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
@@ -631,17 +622,17 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="7" t="s">
         <v>1</v>
@@ -651,7 +642,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>3</v>
@@ -661,7 +652,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -671,7 +662,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -679,7 +670,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
@@ -690,27 +681,24 @@
         <v>6</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>8</v>
@@ -719,16 +707,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65538" spans="2:3" x14ac:dyDescent="0.25">
@@ -740,17 +725,17 @@
     <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F53386-50D9-4EC3-91BA-83D03F08E8F0}">
-  <dimension ref="A2:I65538"/>
+  <dimension ref="A2:H65538"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -761,52 +746,52 @@
     <col min="4" max="5" width="25.1796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.90625" style="2" customWidth="1"/>
     <col min="7" max="7" width="23.90625" style="10" customWidth="1"/>
-    <col min="8" max="9" width="23.90625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="2.1796875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="3"/>
+    <col min="8" max="8" width="23.90625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="2.1796875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
@@ -817,27 +802,24 @@
         <v>6</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>8</v>
@@ -846,16 +828,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="65538" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>